<commit_message>
Reworked TRK adm approach and added MARs to some of the TRK GAM plots
</commit_message>
<xml_diff>
--- a/data/TRK_dates_interpolated_JP.xlsx
+++ b/data/TRK_dates_interpolated_JP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliapop/Desktop/SanJuansPaleo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A8417F-09E7-6A44-ACB0-4E805CA7BAA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD5BEF0-878D-7644-B6A5-722BF5E8CC2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="760" windowWidth="27640" windowHeight="16940" xr2:uid="{9FC5EA70-12F4-7948-9D35-1C4850E93CB1}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{9FC5EA70-12F4-7948-9D35-1C4850E93CB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,24 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={9008DD2A-AFE8-0549-A37E-1CCC3A4F850F}</author>
+  </authors>
+  <commentList>
+    <comment ref="D27" authorId="0" shapeId="0" xr:uid="{9008DD2A-AFE8-0549-A37E-1CCC3A4F850F}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    doesn't add up that 26.7 is higher than 28.5... </t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
@@ -216,7 +234,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -249,6 +267,12 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -294,6 +318,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Julia Pop" id="{02B62E0F-8A92-5745-829E-58F60CE3D758}" userId="S::jupo4408@colorado.edu::72539465-5e3f-4678-afb4-aa340da29f65" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -611,12 +641,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D27" dT="2025-10-28T23:56:28.92" personId="{02B62E0F-8A92-5745-829E-58F60CE3D758}" id="{9008DD2A-AFE8-0549-A37E-1CCC3A4F850F}">
+    <text xml:space="preserve">doesn't add up that 26.7 is higher than 28.5... </text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE34A008-8BEA-1F42-A0C3-3CECE2FCA666}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE34A008-8BEA-1F42-A0C3-3CECE2FCA666}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -635,7 +673,7 @@
     <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="22.33203125" customWidth="1"/>
     <col min="15" max="15" width="25.1640625" customWidth="1"/>
-    <col min="16" max="16" width="21" customWidth="1"/>
+    <col min="16" max="16" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="27.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -724,7 +762,7 @@
         <v>0.13900000000000001</v>
       </c>
       <c r="M2">
-        <f>2025-N2</f>
+        <f t="shared" ref="M2:M8" si="0">2025-N2</f>
         <v>2022.3594731720229</v>
       </c>
       <c r="N2">
@@ -769,7 +807,7 @@
         <v>0.127</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M39" si="0">2025-N3</f>
+        <f t="shared" si="0"/>
         <v>2015.8054314118258</v>
       </c>
       <c r="N3">
@@ -1038,13 +1076,7 @@
         <f>ROUND(J9-J8, 2)</f>
         <v>0.37</v>
       </c>
-      <c r="M9">
-        <f t="shared" si="0"/>
-        <v>1974.0684413883034</v>
-      </c>
-      <c r="N9" s="4">
-        <v>50.931558611696566</v>
-      </c>
+      <c r="N9" s="4"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -1074,13 +1106,7 @@
         <f t="shared" ref="K10:K38" si="2">ROUND(J10-J9, 2)</f>
         <v>0.37</v>
       </c>
-      <c r="M10">
-        <f t="shared" si="0"/>
-        <v>1972.012945882894</v>
-      </c>
-      <c r="N10" s="4">
-        <v>52.987054117105991</v>
-      </c>
+      <c r="N10" s="4"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -1110,13 +1136,7 @@
         <f t="shared" si="2"/>
         <v>0.37</v>
       </c>
-      <c r="M11">
-        <f t="shared" si="0"/>
-        <v>1969.9574503774845</v>
-      </c>
-      <c r="N11" s="4">
-        <v>55.042549622515409</v>
-      </c>
+      <c r="N11" s="4"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -1146,13 +1166,6 @@
         <f t="shared" si="2"/>
         <v>0.37</v>
       </c>
-      <c r="M12">
-        <f t="shared" si="0"/>
-        <v>1967.9019548720751</v>
-      </c>
-      <c r="N12" s="4">
-        <v>57.098045127924827</v>
-      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1182,13 +1195,6 @@
         <f t="shared" si="2"/>
         <v>0.37</v>
       </c>
-      <c r="M13">
-        <f t="shared" si="0"/>
-        <v>1965.8464593666658</v>
-      </c>
-      <c r="N13" s="4">
-        <v>59.153540633334245</v>
-      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1218,13 +1224,6 @@
         <f t="shared" si="2"/>
         <v>0.37</v>
       </c>
-      <c r="M14">
-        <f t="shared" si="0"/>
-        <v>1963.7909638612564</v>
-      </c>
-      <c r="N14" s="4">
-        <v>61.20903613874367</v>
-      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1254,13 +1253,6 @@
         <f t="shared" si="2"/>
         <v>0.37</v>
       </c>
-      <c r="M15">
-        <f t="shared" si="0"/>
-        <v>1961.7354683558469</v>
-      </c>
-      <c r="N15" s="4">
-        <v>63.264531644153088</v>
-      </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1290,13 +1282,6 @@
         <f t="shared" si="2"/>
         <v>0.37</v>
       </c>
-      <c r="M16">
-        <f t="shared" si="0"/>
-        <v>1959.6799728504375</v>
-      </c>
-      <c r="N16" s="4">
-        <v>65.320027149562506</v>
-      </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -1326,13 +1311,6 @@
         <f t="shared" si="2"/>
         <v>0.37</v>
       </c>
-      <c r="M17">
-        <f t="shared" si="0"/>
-        <v>1957.624477345028</v>
-      </c>
-      <c r="N17" s="4">
-        <v>67.375522654971931</v>
-      </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -1362,13 +1340,6 @@
         <f t="shared" si="2"/>
         <v>0.37</v>
       </c>
-      <c r="M18">
-        <f t="shared" si="0"/>
-        <v>1955.5689818396186</v>
-      </c>
-      <c r="N18" s="4">
-        <v>69.431018160381342</v>
-      </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -1398,13 +1369,6 @@
         <f t="shared" si="2"/>
         <v>0.37</v>
       </c>
-      <c r="M19">
-        <f t="shared" si="0"/>
-        <v>1953.5134863342091</v>
-      </c>
-      <c r="N19" s="4">
-        <v>71.486513665790767</v>
-      </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
@@ -1434,13 +1398,7 @@
         <f t="shared" si="2"/>
         <v>0.37</v>
       </c>
-      <c r="M20">
-        <f t="shared" si="0"/>
-        <v>1951.4579908287999</v>
-      </c>
-      <c r="N20" s="4">
-        <v>73.542009171200192</v>
-      </c>
+      <c r="N20" s="4"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -1470,13 +1428,7 @@
         <f t="shared" si="2"/>
         <v>0.37</v>
       </c>
-      <c r="M21">
-        <f t="shared" si="0"/>
-        <v>1949.4024953233904</v>
-      </c>
-      <c r="N21" s="4">
-        <v>75.597504676609617</v>
-      </c>
+      <c r="N21" s="4"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -1506,13 +1458,7 @@
         <f t="shared" si="2"/>
         <v>0.37</v>
       </c>
-      <c r="M22">
-        <f t="shared" si="0"/>
-        <v>1947.346999817981</v>
-      </c>
-      <c r="N22" s="4">
-        <v>77.653000182019028</v>
-      </c>
+      <c r="N22" s="4"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -1542,13 +1488,7 @@
         <f t="shared" si="2"/>
         <v>0.37</v>
       </c>
-      <c r="M23">
-        <f t="shared" si="0"/>
-        <v>1945.2915043125715</v>
-      </c>
-      <c r="N23" s="4">
-        <v>79.708495687428453</v>
-      </c>
+      <c r="N23" s="4"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -1578,13 +1518,7 @@
         <f t="shared" si="2"/>
         <v>0.37</v>
       </c>
-      <c r="M24">
-        <f t="shared" si="0"/>
-        <v>1943.2360088071621</v>
-      </c>
-      <c r="N24" s="4">
-        <v>81.763991192837864</v>
-      </c>
+      <c r="N24" s="4"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
@@ -1614,13 +1548,7 @@
         <f t="shared" si="2"/>
         <v>0.37</v>
       </c>
-      <c r="M25">
-        <f t="shared" si="0"/>
-        <v>1941.1805133017526</v>
-      </c>
-      <c r="N25" s="4">
-        <v>83.819486698247289</v>
-      </c>
+      <c r="N25" s="4"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
@@ -1650,13 +1578,7 @@
         <f t="shared" si="2"/>
         <v>0.37</v>
       </c>
-      <c r="M26">
-        <f t="shared" si="0"/>
-        <v>1939.1250177963434</v>
-      </c>
-      <c r="N26" s="4">
-        <v>85.874982203656714</v>
-      </c>
+      <c r="N26" s="4"/>
     </row>
     <row r="27" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
@@ -1698,7 +1620,7 @@
         <v>0.17100000000000001</v>
       </c>
       <c r="M27">
-        <f t="shared" si="0"/>
+        <f>2025-N27</f>
         <v>1937.0695222909339</v>
       </c>
       <c r="N27" s="3">
@@ -1745,13 +1667,7 @@
         <f t="shared" si="2"/>
         <v>0.52</v>
       </c>
-      <c r="M28">
-        <f t="shared" ref="M28:M38" si="3">2025-N28</f>
-        <v>1934.8308002564675</v>
-      </c>
-      <c r="N28" s="4">
-        <v>90.169199743532502</v>
-      </c>
+      <c r="N28" s="4"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -1784,13 +1700,7 @@
         <f t="shared" si="2"/>
         <v>0.52</v>
       </c>
-      <c r="M29">
-        <f t="shared" si="3"/>
-        <v>1932.5920782220012</v>
-      </c>
-      <c r="N29" s="4">
-        <v>92.407921777998865</v>
-      </c>
+      <c r="N29" s="4"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
@@ -1823,13 +1733,7 @@
         <f t="shared" si="2"/>
         <v>0.52</v>
       </c>
-      <c r="M30">
-        <f t="shared" si="3"/>
-        <v>1930.3533561875347</v>
-      </c>
-      <c r="N30" s="4">
-        <v>94.646643812465214</v>
-      </c>
+      <c r="N30" s="4"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -1862,13 +1766,7 @@
         <f t="shared" si="2"/>
         <v>0.52</v>
       </c>
-      <c r="M31">
-        <f t="shared" si="3"/>
-        <v>1928.1146341530684</v>
-      </c>
-      <c r="N31" s="4">
-        <v>96.885365846931577</v>
-      </c>
+      <c r="N31" s="4"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
@@ -1901,13 +1799,7 @@
         <f t="shared" si="2"/>
         <v>0.52</v>
       </c>
-      <c r="M32">
-        <f t="shared" si="3"/>
-        <v>1925.8759121186022</v>
-      </c>
-      <c r="N32" s="4">
-        <v>99.124087881397941</v>
-      </c>
+      <c r="N32" s="4"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
@@ -1940,13 +1832,7 @@
         <f t="shared" si="2"/>
         <v>0.52</v>
       </c>
-      <c r="M33">
-        <f t="shared" si="3"/>
-        <v>1923.6371900841357</v>
-      </c>
-      <c r="N33" s="4">
-        <v>101.3628099158643</v>
-      </c>
+      <c r="N33" s="4"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
@@ -1980,13 +1866,7 @@
         <v>0.52</v>
       </c>
       <c r="L34" s="2"/>
-      <c r="M34">
-        <f t="shared" si="3"/>
-        <v>1921.3984680496694</v>
-      </c>
-      <c r="N34" s="4">
-        <v>103.60153195033067</v>
-      </c>
+      <c r="N34" s="4"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
@@ -2020,13 +1900,7 @@
         <v>0.52</v>
       </c>
       <c r="L35" s="2"/>
-      <c r="M35">
-        <f t="shared" si="3"/>
-        <v>1919.1597460152029</v>
-      </c>
-      <c r="N35" s="4">
-        <v>105.84025398479702</v>
-      </c>
+      <c r="N35" s="4"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
@@ -2060,13 +1934,7 @@
         <v>0.52</v>
       </c>
       <c r="L36" s="2"/>
-      <c r="M36">
-        <f t="shared" si="3"/>
-        <v>1916.9210239807367</v>
-      </c>
-      <c r="N36" s="4">
-        <v>108.07897601926338</v>
-      </c>
+      <c r="N36" s="4"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
@@ -2100,13 +1968,7 @@
         <v>0.52</v>
       </c>
       <c r="L37" s="2"/>
-      <c r="M37">
-        <f t="shared" si="3"/>
-        <v>1914.6823019462702</v>
-      </c>
-      <c r="N37" s="4">
-        <v>110.31769805372974</v>
-      </c>
+      <c r="N37" s="4"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
@@ -2140,13 +2002,7 @@
         <v>0.52</v>
       </c>
       <c r="L38" s="2"/>
-      <c r="M38">
-        <f t="shared" si="3"/>
-        <v>1912.4435799118039</v>
-      </c>
-      <c r="N38" s="4">
-        <v>112.55642008819609</v>
-      </c>
+      <c r="N38" s="4"/>
     </row>
     <row r="39" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
@@ -2188,7 +2044,7 @@
         <v>0.13900000000000001</v>
       </c>
       <c r="M39">
-        <f t="shared" si="0"/>
+        <f>2025-N39</f>
         <v>1910.2048578773374</v>
       </c>
       <c r="N39" s="3">
@@ -2207,5 +2063,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>